<commit_message>
re-upload to GEO using FASTQ not BAM for CCS
GEO requested that we upload the PacBio CCSs
in FASTQ files rather than BAM files, so doing
that with this commit.
</commit_message>
<xml_diff>
--- a/GEO_upload/metadata.xlsx
+++ b/GEO_upload/metadata.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="148">
   <si>
     <t># High-throughput sequencing metadata template (version 2.1).</t>
   </si>
@@ -340,10 +340,13 @@
     <t>single or paired-end</t>
   </si>
   <si>
-    <t>BAM file with PacBio CCSs</t>
-  </si>
-  <si>
-    <t>268c776fa5f778e2bf70f9bc1dd7fcf3</t>
+    <t>2017-06-08_ccs.fastq.gz</t>
+  </si>
+  <si>
+    <t>FASTQ file with PacBio CCSs</t>
+  </si>
+  <si>
+    <t>e19c98ff793be4685595b584531ed36b</t>
   </si>
   <si>
     <t>PacBio Sequel</t>
@@ -355,37 +358,55 @@
     <t>26d1727811f15b380fc0bd26630e8898</t>
   </si>
   <si>
-    <t>616b40a6f52cb4f6eb81e54b15a90ad5</t>
+    <t>2017-12-07_ccs.fastq.gz</t>
+  </si>
+  <si>
+    <t>8fde9acce7dc5f4db84b6b8a9fbb36c3</t>
   </si>
   <si>
     <t>f3ef600db9558a3325ac7e1c02514778</t>
   </si>
   <si>
-    <t>d18b8a3bb52263b4de4c19086c221a58</t>
+    <t>2018-06-22_nonPol_ccs.fastq.gz</t>
+  </si>
+  <si>
+    <t>5674846b3243c125af2245b2a84bd7d0</t>
   </si>
   <si>
     <t>91a15217144bc02200852e7d14a08500</t>
   </si>
   <si>
-    <t>9800607e16fe10619d099bf82bddaa8e</t>
+    <t>2018-06-22_Pol-1_ccs.fastq.gz</t>
+  </si>
+  <si>
+    <t>2660b4ab498f6c8dfebadad5cdc0800b</t>
   </si>
   <si>
     <t>a5f9198420a5a536e2d5c2b8234ecdef</t>
   </si>
   <si>
-    <t>ee87cd382b06418ff85496ad208f46bb</t>
+    <t>2018-06-22_Pol-2_ccs.fastq.gz</t>
+  </si>
+  <si>
+    <t>25ac56328cfb8945bc38258886db42a8</t>
   </si>
   <si>
     <t>bfb7b0da4a910784d894f2b30e80e7a8</t>
   </si>
   <si>
-    <t>1fb9dbac3404ef7b4507b9379f6120b5</t>
+    <t>2018-06-22_Pol_open_ccs.fastq.gz</t>
+  </si>
+  <si>
+    <t>3fc3561ece838cbfbdd42973bf6769d8</t>
   </si>
   <si>
     <t>3377e205e5534c585be7d1844259a369</t>
   </si>
   <si>
-    <t>69cbaa0beecc987a0f4b5642e738ad1c</t>
+    <t>2018-08-08_Pol_circ_ccs.fastq.gz</t>
+  </si>
+  <si>
+    <t>b2c563048a230070895e4dde0565b9aa</t>
   </si>
   <si>
     <t>54c62f99e5960f5e498e95e7a17f2d6d</t>
@@ -444,7 +465,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="16">
+  <fonts count="14">
     <font>
       <name val="Arial"/>
       <sz val="10"/>
@@ -478,20 +499,6 @@
       <b val="1"/>
       <color indexed="10"/>
       <sz val="10"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <family val="2"/>
-      <b val="1"/>
-      <color indexed="8"/>
-      <sz val="8"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <family val="2"/>
-      <b val="1"/>
-      <color indexed="81"/>
-      <sz val="8"/>
     </font>
     <font>
       <name val="Tahoma"/>
@@ -592,8 +599,8 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="10" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
@@ -621,14 +628,14 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="3" fontId="10" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="3" fontId="12" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="3" fontId="11" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="13" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="3" fontId="12" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="3" fontId="14" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="3" fontId="13" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="15" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="4" fontId="12" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="15" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="0" fillId="4" fontId="10" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="13" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
@@ -1392,7 +1399,7 @@
   <dimension ref="A1:AE241"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="F73" sqref="F73"/>
+      <selection activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="28.6640625" defaultRowHeight="13" outlineLevelCol="0"/>
@@ -2055,16 +2062,16 @@
     </row>
     <row customFormat="1" customHeight="1" ht="14" r="56" s="34" spans="1:31">
       <c r="A56" s="33" t="s">
-        <v>43</v>
+        <v>108</v>
       </c>
       <c r="B56" s="34" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C56" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D56" s="34" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row customFormat="1" customHeight="1" ht="28" r="57" s="34" spans="1:31">
@@ -2072,27 +2079,27 @@
         <v>44</v>
       </c>
       <c r="B57" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="C57" t="s">
+        <v>113</v>
+      </c>
+      <c r="D57" s="34" t="s">
         <v>111</v>
-      </c>
-      <c r="C57" t="s">
-        <v>112</v>
-      </c>
-      <c r="D57" s="34" t="s">
-        <v>110</v>
       </c>
     </row>
     <row customFormat="1" customHeight="1" ht="14" r="58" s="34" spans="1:31">
       <c r="A58" s="33" t="s">
-        <v>45</v>
+        <v>114</v>
       </c>
       <c r="B58" s="34" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C58" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D58" s="34" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row customFormat="1" customHeight="1" ht="28" r="59" s="34" spans="1:31">
@@ -2100,28 +2107,28 @@
         <v>46</v>
       </c>
       <c r="B59" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="C59" t="s">
+        <v>116</v>
+      </c>
+      <c r="D59" s="34" t="s">
         <v>111</v>
-      </c>
-      <c r="C59" t="s">
-        <v>114</v>
-      </c>
-      <c r="D59" s="34" t="s">
-        <v>110</v>
       </c>
       <c r="L59" s="33" t="n"/>
     </row>
     <row customFormat="1" customHeight="1" ht="14" r="60" s="34" spans="1:31">
       <c r="A60" s="33" t="s">
-        <v>47</v>
+        <v>117</v>
       </c>
       <c r="B60" s="34" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C60" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="D60" s="34" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="K60" s="33" t="n"/>
       <c r="L60" s="33" t="n"/>
@@ -2131,13 +2138,13 @@
         <v>48</v>
       </c>
       <c r="B61" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="C61" t="s">
+        <v>119</v>
+      </c>
+      <c r="D61" s="34" t="s">
         <v>111</v>
-      </c>
-      <c r="C61" t="s">
-        <v>116</v>
-      </c>
-      <c r="D61" s="34" t="s">
-        <v>110</v>
       </c>
       <c r="J61" s="33" t="n"/>
       <c r="K61" s="33" t="n"/>
@@ -2145,16 +2152,16 @@
     </row>
     <row customFormat="1" customHeight="1" ht="14" r="62" s="34" spans="1:31">
       <c r="A62" s="33" t="s">
-        <v>49</v>
+        <v>120</v>
       </c>
       <c r="B62" s="34" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C62" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="D62" s="34" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="I62" s="33" t="n"/>
       <c r="J62" s="33" t="n"/>
@@ -2166,13 +2173,13 @@
         <v>50</v>
       </c>
       <c r="B63" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="C63" t="s">
+        <v>122</v>
+      </c>
+      <c r="D63" s="34" t="s">
         <v>111</v>
-      </c>
-      <c r="C63" t="s">
-        <v>118</v>
-      </c>
-      <c r="D63" s="34" t="s">
-        <v>110</v>
       </c>
       <c r="H63" s="33" t="n"/>
       <c r="I63" s="33" t="n"/>
@@ -2182,16 +2189,16 @@
     </row>
     <row customFormat="1" customHeight="1" ht="14" r="64" s="34" spans="1:31">
       <c r="A64" s="33" t="s">
-        <v>51</v>
+        <v>123</v>
       </c>
       <c r="B64" s="34" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C64" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="D64" s="34" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G64" s="33" t="n"/>
       <c r="H64" s="33" t="n"/>
@@ -2205,13 +2212,13 @@
         <v>52</v>
       </c>
       <c r="B65" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="C65" t="s">
+        <v>125</v>
+      </c>
+      <c r="D65" s="34" t="s">
         <v>111</v>
-      </c>
-      <c r="C65" t="s">
-        <v>120</v>
-      </c>
-      <c r="D65" s="34" t="s">
-        <v>110</v>
       </c>
       <c r="F65" s="33" t="n"/>
       <c r="G65" s="33" t="n"/>
@@ -2223,16 +2230,16 @@
     </row>
     <row customFormat="1" customHeight="1" ht="14" r="66" s="34" spans="1:31">
       <c r="A66" s="33" t="s">
-        <v>53</v>
+        <v>126</v>
       </c>
       <c r="B66" s="34" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C66" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="D66" s="34" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E66" s="33" t="n"/>
       <c r="F66" s="33" t="n"/>
@@ -2248,13 +2255,13 @@
         <v>54</v>
       </c>
       <c r="B67" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="C67" t="s">
+        <v>128</v>
+      </c>
+      <c r="D67" s="34" t="s">
         <v>111</v>
-      </c>
-      <c r="C67" t="s">
-        <v>122</v>
-      </c>
-      <c r="D67" s="34" t="s">
-        <v>110</v>
       </c>
       <c r="E67" s="33" t="n"/>
       <c r="F67" s="33" t="n"/>
@@ -2267,16 +2274,16 @@
     </row>
     <row customFormat="1" customHeight="1" ht="14" r="68" s="34" spans="1:31">
       <c r="A68" s="33" t="s">
-        <v>55</v>
+        <v>129</v>
       </c>
       <c r="B68" s="34" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C68" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="D68" s="34" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E68" s="33" t="n"/>
       <c r="F68" s="33" t="n"/>
@@ -2292,13 +2299,13 @@
         <v>56</v>
       </c>
       <c r="B69" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="C69" t="s">
+        <v>131</v>
+      </c>
+      <c r="D69" s="34" t="s">
         <v>111</v>
-      </c>
-      <c r="C69" t="s">
-        <v>124</v>
-      </c>
-      <c r="D69" s="34" t="s">
-        <v>110</v>
       </c>
       <c r="E69" s="33" t="n"/>
       <c r="F69" s="33" t="n"/>
@@ -2314,16 +2321,16 @@
         <v>57</v>
       </c>
       <c r="B70" s="34" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="C70" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="D70" s="34" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="E70" s="33" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="F70" s="33" t="n"/>
       <c r="G70" s="33" t="n"/>
@@ -2338,16 +2345,16 @@
         <v>58</v>
       </c>
       <c r="B71" s="34" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="C71" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="D71" s="34" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="E71" s="33" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="F71" s="33" t="n"/>
       <c r="G71" s="33" t="n"/>
@@ -2362,16 +2369,16 @@
         <v>59</v>
       </c>
       <c r="B72" s="34" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="C72" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="D72" s="34" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="E72" s="33" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="F72" s="33" t="n"/>
       <c r="G72" s="33" t="n"/>
@@ -2383,26 +2390,26 @@
     </row>
     <row customFormat="1" r="73" s="25" spans="1:31">
       <c r="A73" s="25" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
     </row>
     <row customFormat="1" r="74" s="24" spans="1:31">
       <c r="A74" s="29" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
     </row>
     <row customFormat="1" r="75" s="27" spans="1:31">
       <c r="A75" s="27" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="B75" s="27" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="C75" s="30" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="D75" s="27" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
     </row>
     <row customFormat="1" r="76" s="24" spans="1:31"/>

</xml_diff>